<commit_message>
adb xls export improvements
- list xls translations
- set default font and fontsize in templates
- keyfields

Change-Id: I343eb123d658f688c3981cf42726c45386ecd853
Reviewed-on: http://gerrit.tine20.com/customers/8625
Tested-by: Jenkins CI (http://ci.tine20.com/) <tine20-jenkins@metaways.de>
Reviewed-by: Cornelius Weiss <c.weiss@metaways.de>
</commit_message>
<xml_diff>
--- a/tine20/Addressbook/Export/templates/addressbook_contact_export.xlsx
+++ b/tine20/Addressbook/Export/templates/addressbook_contact_export.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28502"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pzornsch/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nelius/src/tine20.git/tine20/Addressbook/Export/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCCFACD-C900-6047-ACEF-DED76E844B03}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4400" yWindow="2780" windowWidth="20620" windowHeight="13220" tabRatio="500"/>
+    <workbookView xWindow="4400" yWindow="2780" windowWidth="24400" windowHeight="13220" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -38,14 +39,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="8"/>
@@ -138,7 +138,7 @@
   <cellStyles count="3">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -214,6 +214,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -228,14 +231,20 @@
       <xdr:rowOff>35491</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>554683</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>241802</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>517075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Bild 2" descr="${twig:branding.logo}"/>
+        <xdr:cNvPr id="3" name="Bild 2" descr="${twig:branding.logo}">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -529,17 +538,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="110" zoomScaleNormal="110" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="7" width="8.83203125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="7" width="9" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="44" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>